<commit_message>
json to excel, reinicio de entradas post registro
</commit_message>
<xml_diff>
--- a/data/presupuesto.xlsx
+++ b/data/presupuesto.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,6 +508,56 @@
       <c r="E3" t="inlineStr">
         <is>
           <t>2025-05-05</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ingreso</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Otros</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>transferencia</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2675</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Ingreso</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Inversiones</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>nu 14% 3 meses</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>766</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
         </is>
       </c>
     </row>
@@ -522,7 +572,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -607,6 +657,81 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Egreso</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Vivienda</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>servicio de gas</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>550</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Egreso</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Salud</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>medicamentos</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1250</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Egreso</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Alimentos</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>café</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>360</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025-05-06</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>